<commit_message>
resolved second point, started third point (sbrt')
</commit_message>
<xml_diff>
--- a/FirstPart/Greenhouse/data_greenhouse.xlsx
+++ b/FirstPart/Greenhouse/data_greenhouse.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Desktop\Magistrale\SecondoSemestre\IndustrialAutomation\Exercises\Greenhouse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Desktop\Magistrale\SecondoSemestre\IndustrialAutomation\Projects\Industrial-Automation-Projects\FirstPart\Greenhouse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BDC07B-DECA-493D-B2B3-44B7C04C0075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23BCC12-D3C5-485F-AF53-88CCC78DC04E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{34C2F785-5D4F-4160-99D8-F523D479713D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11712" windowHeight="12240" xr2:uid="{34C2F785-5D4F-4160-99D8-F523D479713D}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,24 +36,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>time</t>
   </si>
   <si>
-    <t>track K</t>
-  </si>
-  <si>
     <t>ext K</t>
-  </si>
-  <si>
-    <t>track °C</t>
   </si>
   <si>
     <t>ext °C</t>
   </si>
   <si>
     <t>radiation</t>
+  </si>
+  <si>
+    <t>track_m1 °C</t>
+  </si>
+  <si>
+    <t>track_m1 K</t>
+  </si>
+  <si>
+    <t>track_m2 °C</t>
+  </si>
+  <si>
+    <t>track_m2 K</t>
   </si>
 </sst>
 </file>
@@ -95,9 +101,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -434,37 +438,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9F7AEFF-8D72-4974-97AC-1332C8CB85D0}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
@@ -478,539 +488,714 @@
         <v>18</v>
       </c>
       <c r="F2">
-        <f>273+E2</f>
+        <f t="shared" ref="F2:F26" si="0">273+E2</f>
         <v>291</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <f>273+I2</f>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
-      <c r="C3" s="2">
-        <f t="shared" ref="C3:C26" si="0">273+B3</f>
+      <c r="C3">
+        <f t="shared" ref="C3:C26" si="1">273+B3</f>
         <v>283</v>
       </c>
       <c r="E3">
         <v>18</v>
       </c>
-      <c r="F3" s="2">
-        <f>273+E3</f>
+      <c r="F3">
+        <f t="shared" si="0"/>
         <v>291</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J26" si="2">273+I3</f>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
         <v>10</v>
       </c>
-      <c r="C4" s="2">
-        <f t="shared" si="0"/>
+      <c r="C4">
+        <f t="shared" si="1"/>
         <v>283</v>
       </c>
       <c r="E4">
         <v>18</v>
       </c>
-      <c r="F4" s="2">
-        <f>273+E4</f>
+      <c r="F4">
+        <f t="shared" si="0"/>
         <v>291</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="2"/>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
         <v>10</v>
       </c>
-      <c r="C5" s="2">
-        <f t="shared" si="0"/>
+      <c r="C5">
+        <f t="shared" si="1"/>
         <v>283</v>
       </c>
       <c r="E5">
         <v>18</v>
       </c>
-      <c r="F5" s="2">
-        <f>273+E5</f>
+      <c r="F5">
+        <f t="shared" si="0"/>
         <v>291</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="2"/>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
         <v>10</v>
       </c>
-      <c r="C6" s="2">
-        <f t="shared" si="0"/>
+      <c r="C6">
+        <f t="shared" si="1"/>
         <v>283</v>
       </c>
       <c r="E6">
         <v>17</v>
       </c>
-      <c r="F6" s="2">
-        <f>273+E6</f>
+      <c r="F6">
+        <f t="shared" si="0"/>
         <v>290</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="2"/>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
         <v>10</v>
       </c>
-      <c r="C7" s="2">
-        <f t="shared" si="0"/>
+      <c r="C7">
+        <f t="shared" si="1"/>
         <v>283</v>
       </c>
       <c r="E7">
         <v>17</v>
       </c>
-      <c r="F7" s="2">
-        <f>273+E7</f>
+      <c r="F7">
+        <f t="shared" si="0"/>
         <v>290</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
         <v>10</v>
       </c>
-      <c r="C8" s="2">
-        <f t="shared" si="0"/>
+      <c r="C8">
+        <f t="shared" si="1"/>
         <v>283</v>
       </c>
       <c r="E8">
         <v>17</v>
       </c>
-      <c r="F8" s="2">
-        <f>273+E8</f>
+      <c r="F8">
+        <f t="shared" si="0"/>
         <v>290</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+      <c r="I8">
+        <v>10</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="2"/>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
         <v>10</v>
       </c>
-      <c r="C9" s="2">
-        <f t="shared" si="0"/>
+      <c r="C9">
+        <f t="shared" si="1"/>
         <v>283</v>
       </c>
       <c r="E9">
         <v>17</v>
       </c>
-      <c r="F9" s="2">
-        <f>273+E9</f>
+      <c r="F9">
+        <f t="shared" si="0"/>
         <v>290</v>
       </c>
       <c r="H9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+      <c r="I9">
+        <v>10</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="2"/>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
         <v>10</v>
       </c>
-      <c r="C10" s="2">
-        <f t="shared" si="0"/>
+      <c r="C10">
+        <f t="shared" si="1"/>
         <v>283</v>
       </c>
       <c r="E10">
         <v>17</v>
       </c>
-      <c r="F10" s="2">
-        <f>273+E10</f>
+      <c r="F10">
+        <f t="shared" si="0"/>
         <v>290</v>
       </c>
       <c r="H10">
         <v>136</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="I10">
+        <v>10</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="2"/>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
-      <c r="C11" s="2">
-        <f t="shared" si="0"/>
+      <c r="C11">
+        <f t="shared" si="1"/>
         <v>283</v>
       </c>
       <c r="E11">
         <v>19</v>
       </c>
-      <c r="F11" s="2">
-        <f>273+E11</f>
+      <c r="F11">
+        <f t="shared" si="0"/>
         <v>292</v>
       </c>
       <c r="H11">
         <v>325</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="2"/>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
         <v>5</v>
       </c>
-      <c r="C12" s="2">
-        <f t="shared" si="0"/>
+      <c r="C12">
+        <f t="shared" si="1"/>
         <v>278</v>
       </c>
       <c r="E12">
         <v>20</v>
       </c>
-      <c r="F12" s="2">
-        <f>273+E12</f>
+      <c r="F12">
+        <f t="shared" si="0"/>
         <v>293</v>
       </c>
       <c r="H12">
         <v>502</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+      <c r="I12">
+        <v>8</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="2"/>
+        <v>281</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>11</v>
       </c>
       <c r="B13">
         <v>5</v>
       </c>
-      <c r="C13" s="2">
-        <f t="shared" si="0"/>
+      <c r="C13">
+        <f t="shared" si="1"/>
         <v>278</v>
       </c>
       <c r="E13">
         <v>21</v>
       </c>
-      <c r="F13" s="2">
-        <f>273+E13</f>
+      <c r="F13">
+        <f t="shared" si="0"/>
         <v>294</v>
       </c>
       <c r="H13">
         <v>497</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+      <c r="I13">
+        <v>8</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="2"/>
+        <v>281</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14">
         <v>12</v>
       </c>
       <c r="B14">
         <v>10</v>
       </c>
-      <c r="C14" s="2">
-        <f t="shared" si="0"/>
+      <c r="C14">
+        <f t="shared" si="1"/>
         <v>283</v>
       </c>
       <c r="E14">
         <v>22</v>
       </c>
-      <c r="F14" s="2">
-        <f>273+E14</f>
+      <c r="F14">
+        <f t="shared" si="0"/>
         <v>295</v>
       </c>
       <c r="H14">
         <v>452</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+      <c r="I14">
+        <v>15</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="2"/>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>13</v>
       </c>
       <c r="B15">
         <v>10</v>
       </c>
-      <c r="C15" s="2">
-        <f t="shared" si="0"/>
+      <c r="C15">
+        <f t="shared" si="1"/>
         <v>283</v>
       </c>
       <c r="E15">
         <v>22</v>
       </c>
-      <c r="F15" s="2">
-        <f>273+E15</f>
+      <c r="F15">
+        <f t="shared" si="0"/>
         <v>295</v>
       </c>
       <c r="H15">
         <v>623</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
+      <c r="I15">
+        <v>15</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="2"/>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>14</v>
       </c>
       <c r="B16">
         <v>10</v>
       </c>
-      <c r="C16" s="2">
-        <f t="shared" si="0"/>
+      <c r="C16">
+        <f t="shared" si="1"/>
         <v>283</v>
       </c>
       <c r="E16">
         <v>22</v>
       </c>
-      <c r="F16" s="2">
-        <f>273+E16</f>
+      <c r="F16">
+        <f t="shared" si="0"/>
         <v>295</v>
       </c>
       <c r="H16">
         <v>765</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
+      <c r="I16">
+        <v>15</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="2"/>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17">
         <v>15</v>
       </c>
       <c r="B17">
         <v>9</v>
       </c>
-      <c r="C17" s="2">
-        <f t="shared" si="0"/>
+      <c r="C17">
+        <f t="shared" si="1"/>
         <v>282</v>
       </c>
       <c r="E17">
         <v>22</v>
       </c>
-      <c r="F17" s="2">
-        <f>273+E17</f>
+      <c r="F17">
+        <f t="shared" si="0"/>
         <v>295</v>
       </c>
       <c r="H17">
         <v>735</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+      <c r="I17">
+        <v>13</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="2"/>
+        <v>286</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>16</v>
       </c>
       <c r="B18">
         <v>8</v>
       </c>
-      <c r="C18" s="2">
-        <f t="shared" si="0"/>
+      <c r="C18">
+        <f t="shared" si="1"/>
         <v>281</v>
       </c>
       <c r="E18">
         <v>22</v>
       </c>
-      <c r="F18" s="2">
-        <f>273+E18</f>
+      <c r="F18">
+        <f t="shared" si="0"/>
         <v>295</v>
       </c>
       <c r="H18">
         <v>626</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
+      <c r="I18">
+        <v>14</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="2"/>
+        <v>287</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>17</v>
       </c>
       <c r="B19">
         <v>7</v>
       </c>
-      <c r="C19" s="2">
-        <f t="shared" si="0"/>
+      <c r="C19">
+        <f t="shared" si="1"/>
         <v>280</v>
       </c>
       <c r="E19">
         <v>21</v>
       </c>
-      <c r="F19" s="2">
-        <f>273+E19</f>
+      <c r="F19">
+        <f t="shared" si="0"/>
         <v>294</v>
       </c>
       <c r="H19">
         <v>474</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
+      <c r="I19">
+        <v>14</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="2"/>
+        <v>287</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20">
         <v>18</v>
       </c>
       <c r="B20">
         <v>7</v>
       </c>
-      <c r="C20" s="2">
-        <f t="shared" si="0"/>
+      <c r="C20">
+        <f t="shared" si="1"/>
         <v>280</v>
       </c>
       <c r="E20">
         <v>21</v>
       </c>
-      <c r="F20" s="2">
-        <f>273+E20</f>
+      <c r="F20">
+        <f t="shared" si="0"/>
         <v>294</v>
       </c>
       <c r="H20">
         <v>293</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
+      <c r="I20">
+        <v>8</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="2"/>
+        <v>281</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21">
         <v>19</v>
       </c>
       <c r="B21">
         <v>7</v>
       </c>
-      <c r="C21" s="2">
-        <f t="shared" si="0"/>
+      <c r="C21">
+        <f t="shared" si="1"/>
         <v>280</v>
       </c>
       <c r="E21">
         <v>20</v>
       </c>
-      <c r="F21" s="2">
-        <f>273+E21</f>
+      <c r="F21">
+        <f t="shared" si="0"/>
         <v>293</v>
       </c>
       <c r="H21">
         <v>107</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
+      <c r="I21">
+        <v>8</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="2"/>
+        <v>281</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22">
         <v>20</v>
       </c>
       <c r="B22">
         <v>7</v>
       </c>
-      <c r="C22" s="2">
-        <f t="shared" si="0"/>
+      <c r="C22">
+        <f t="shared" si="1"/>
         <v>280</v>
       </c>
       <c r="E22">
         <v>20</v>
       </c>
-      <c r="F22" s="2">
-        <f>273+E22</f>
+      <c r="F22">
+        <f t="shared" si="0"/>
         <v>293</v>
       </c>
       <c r="H22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
+      <c r="I22">
+        <v>5</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="2"/>
+        <v>278</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23">
         <v>21</v>
       </c>
       <c r="B23">
         <v>6</v>
       </c>
-      <c r="C23" s="2">
-        <f t="shared" si="0"/>
+      <c r="C23">
+        <f t="shared" si="1"/>
         <v>279</v>
       </c>
       <c r="E23">
         <v>19</v>
       </c>
-      <c r="F23" s="2">
-        <f>273+E23</f>
+      <c r="F23">
+        <f t="shared" si="0"/>
         <v>292</v>
       </c>
       <c r="H23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
+      <c r="I23">
+        <v>4</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="2"/>
+        <v>277</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24">
         <v>22</v>
       </c>
       <c r="B24">
         <v>10</v>
       </c>
-      <c r="C24" s="2">
-        <f t="shared" si="0"/>
+      <c r="C24">
+        <f t="shared" si="1"/>
         <v>283</v>
       </c>
       <c r="E24">
         <v>18</v>
       </c>
-      <c r="F24" s="2">
-        <f>273+E24</f>
+      <c r="F24">
+        <f t="shared" si="0"/>
         <v>291</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
+      <c r="I24">
+        <v>10</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="2"/>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25">
         <v>23</v>
       </c>
       <c r="B25">
         <v>10</v>
       </c>
-      <c r="C25" s="2">
-        <f t="shared" si="0"/>
+      <c r="C25">
+        <f t="shared" si="1"/>
         <v>283</v>
       </c>
       <c r="E25">
         <v>18</v>
       </c>
-      <c r="F25" s="2">
-        <f>273+E25</f>
+      <c r="F25">
+        <f t="shared" si="0"/>
         <v>291</v>
       </c>
       <c r="H25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
+      <c r="I25">
+        <v>10</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="2"/>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26">
         <v>24</v>
       </c>
       <c r="B26">
         <v>10</v>
       </c>
-      <c r="C26" s="2">
-        <f t="shared" si="0"/>
+      <c r="C26">
+        <f t="shared" si="1"/>
         <v>283</v>
       </c>
       <c r="E26">
         <v>17</v>
       </c>
-      <c r="F26" s="2">
-        <f>273+E26</f>
+      <c r="F26">
+        <f t="shared" si="0"/>
         <v>290</v>
       </c>
       <c r="H26">
         <v>0</v>
+      </c>
+      <c r="I26">
+        <v>10</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="2"/>
+        <v>283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>